<commit_message>
added instructions and modified some columns
</commit_message>
<xml_diff>
--- a/Templates/Purchased_Electricity.xlsx
+++ b/Templates/Purchased_Electricity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AI\LevelUPESG\Batch-input-Page\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2FD2D0-6126-4515-B842-69AB368C091B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD9CFDB-65BC-4CBD-A831-2C06FB90A0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3931B47E-5CA9-47BA-869F-3C1FD779CCC4}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{3931B47E-5CA9-47BA-869F-3C1FD779CCC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Purchased Electricity" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="638">
   <si>
     <t>Asset Name</t>
   </si>
@@ -1847,9 +1847,6 @@
     <t>ZWD</t>
   </si>
   <si>
-    <t>Actual / Estimated</t>
-  </si>
-  <si>
     <t>company</t>
   </si>
   <si>
@@ -1868,24 +1865,6 @@
     <t>company5</t>
   </si>
   <si>
-    <t>company6</t>
-  </si>
-  <si>
-    <t>company7</t>
-  </si>
-  <si>
-    <t>company8</t>
-  </si>
-  <si>
-    <t>company9</t>
-  </si>
-  <si>
-    <t>company10</t>
-  </si>
-  <si>
-    <t>company11</t>
-  </si>
-  <si>
     <t>The fiscal year for which the data is being reported, e.g., 2021</t>
   </si>
   <si>
@@ -1899,6 +1878,69 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Actual/Estimated</t>
+  </si>
+  <si>
+    <t>Indicates whether the reported data is an actual measurement or an estimate.</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>reason 1</t>
+  </si>
+  <si>
+    <t>link l</t>
+  </si>
+  <si>
+    <t>reason 2</t>
+  </si>
+  <si>
+    <t>link 2</t>
+  </si>
+  <si>
+    <t>reason 3</t>
+  </si>
+  <si>
+    <t>reason 4</t>
+  </si>
+  <si>
+    <t>link 3</t>
+  </si>
+  <si>
+    <t>The country in which the electricity is consumed</t>
+  </si>
+  <si>
+    <t>The pricing structure applied to the electricity consumption. It details how the electricity is billed to the consumer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The type of value being recorded, such as Consumption or Total Spend </t>
+  </si>
+  <si>
+    <t>The total amount of electricity consumed during the reporting period, measured in kilowatt-hours (kWh)</t>
+  </si>
+  <si>
+    <t>The total cost associated with the asset for the reporting period</t>
+  </si>
+  <si>
+    <t>The currency in which the total spend is reported</t>
+  </si>
+  <si>
+    <t>The share of each energy type in the total electricity consumed</t>
+  </si>
+  <si>
+    <t>Any other fuel types contributing to the energy mix not covered by the categories above</t>
+  </si>
+  <si>
+    <t>The proportion of electricity generated from renewable sources such as solar, wind, hydro, or biomass</t>
+  </si>
+  <si>
+    <t>The percentage of electricity sourced from nuclear power</t>
+  </si>
+  <si>
+    <t>The share of electricity produced from natural gas</t>
   </si>
 </sst>
 </file>
@@ -1960,7 +2002,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="2" tint="-0.499984740745262"/>
@@ -2074,31 +2126,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9F0D4CA6-F7F4-45CA-A02E-33E2987DEEC0}" name="Table7" displayName="Table7" ref="A1:V1683" totalsRowShown="0" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9F0D4CA6-F7F4-45CA-A02E-33E2987DEEC0}" name="Table7" displayName="Table7" ref="A1:V1683" totalsRowShown="0" dataDxfId="26">
   <autoFilter ref="A1:V1683" xr:uid="{9F0D4CA6-F7F4-45CA-A02E-33E2987DEEC0}"/>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{1E140E37-E478-4AA7-A20E-C89F7450FCE2}" name="Asset Name" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{5A319E75-01D6-4812-AB3A-812976120A4D}" name="Asset Type" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{F26AA676-CF15-43F7-BC0B-D92AB0C22EBF}" name="Country" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{0559A132-E90C-4372-96D8-169B6B2D7F5F}" name="Reporting Year" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{ABA97DDC-FE81-4041-86D7-71ABA38BCAF1}" name="Tariff" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{3272EB4B-9B6E-4A66-A6D9-DAA423B2D6E5}" name="Value Type" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{5C22D143-129C-4741-B2B0-6E7995162F95}" name="Consumption (kWh)" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{E6241F5F-738A-4111-90E1-521F3060E586}" name="Total Spend" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{D476D0EA-C319-454D-A157-14872ACDB843}" name="Currency" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{1546B72B-1EFF-4247-8A7D-88E612BB1E69}" name="Actual / Estimated" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{66FAC7A4-DDE7-4406-809F-81E419FB9484}" name="Coal" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{CC2C9114-3249-46CB-9566-7446D34A6478}" name="Coal Percent" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{D1BA01D8-B969-4119-B170-29C8EF2EC7F0}" name="Natural Gas" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{B1AB1D4A-B663-4EA2-8C74-E308481EDA2C}" name="Natural Gas percent" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{221CC043-F993-4AA8-BCEA-6E9C3D11C974}" name="Nuclear" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{4FB4046A-F772-4C0B-B7A3-C273B81B3121}" name="Nuclear percent" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{A10D2298-958E-4309-A58A-1B087E459CBB}" name="Renewables" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{160C808E-F115-430E-B8EB-A43DF9A84066}" name="Renewables percent" dataDxfId="7"/>
-    <tableColumn id="19" xr3:uid="{8CDD6B8F-FC5B-461B-9AAA-E5D717021003}" name="Other Fuel" dataDxfId="6"/>
-    <tableColumn id="20" xr3:uid="{C7DBF4F7-BA0C-4C60-A1F7-EF14DB869191}" name="Other Fuel percent" dataDxfId="5"/>
-    <tableColumn id="21" xr3:uid="{4E22ED4F-BB3B-4C70-8495-266CE22774D9}" name="Assumption basis" dataDxfId="4"/>
-    <tableColumn id="22" xr3:uid="{CC5E3CB3-3395-43B1-865A-F195D64EC842}" name="Evidence" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{1E140E37-E478-4AA7-A20E-C89F7450FCE2}" name="Asset Name" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{5A319E75-01D6-4812-AB3A-812976120A4D}" name="Asset Type" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{F26AA676-CF15-43F7-BC0B-D92AB0C22EBF}" name="Country" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{0559A132-E90C-4372-96D8-169B6B2D7F5F}" name="Reporting Year" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{ABA97DDC-FE81-4041-86D7-71ABA38BCAF1}" name="Tariff" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{3272EB4B-9B6E-4A66-A6D9-DAA423B2D6E5}" name="Value Type" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{5C22D143-129C-4741-B2B0-6E7995162F95}" name="Consumption (kWh)" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{E6241F5F-738A-4111-90E1-521F3060E586}" name="Total Spend" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{D476D0EA-C319-454D-A157-14872ACDB843}" name="Currency" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{66FAC7A4-DDE7-4406-809F-81E419FB9484}" name="Coal" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{CC2C9114-3249-46CB-9566-7446D34A6478}" name="Coal Percent" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{D1BA01D8-B969-4119-B170-29C8EF2EC7F0}" name="Natural Gas" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{B1AB1D4A-B663-4EA2-8C74-E308481EDA2C}" name="Natural Gas percent" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{221CC043-F993-4AA8-BCEA-6E9C3D11C974}" name="Nuclear" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{4FB4046A-F772-4C0B-B7A3-C273B81B3121}" name="Nuclear percent" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{A10D2298-958E-4309-A58A-1B087E459CBB}" name="Renewables" dataDxfId="10"/>
+    <tableColumn id="18" xr3:uid="{160C808E-F115-430E-B8EB-A43DF9A84066}" name="Renewables percent" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{8CDD6B8F-FC5B-461B-9AAA-E5D717021003}" name="Other Fuel" dataDxfId="8"/>
+    <tableColumn id="20" xr3:uid="{C7DBF4F7-BA0C-4C60-A1F7-EF14DB869191}" name="Other Fuel percent" dataDxfId="7"/>
+    <tableColumn id="23" xr3:uid="{D65BDEC1-CF3C-4940-BECF-B59F4C05CCCA}" name="Actual/Estimated" dataDxfId="4"/>
+    <tableColumn id="21" xr3:uid="{4E22ED4F-BB3B-4C70-8495-266CE22774D9}" name="Assumption basis" dataDxfId="6"/>
+    <tableColumn id="22" xr3:uid="{CC5E3CB3-3395-43B1-865A-F195D64EC842}" name="Evidence" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2460,8 +2512,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V1683"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2470,22 +2522,22 @@
     <col min="2" max="2" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.21875" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.6640625" customWidth="1"/>
     <col min="21" max="21" width="24.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="9.109375" style="2"/>
@@ -2520,37 +2572,37 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>606</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
         <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>617</v>
       </c>
       <c r="U1" t="s">
         <v>19</v>
@@ -2559,7 +2611,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="1" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="1" customFormat="1" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -2567,54 +2619,90 @@
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>210</v>
+        <v>627</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="G2" s="1">
-        <v>524245</v>
-      </c>
-      <c r="H2" s="1">
-        <v>20000</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>628</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>629</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>631</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>618</v>
       </c>
       <c r="U2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="D3" s="4">
         <v>2023</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>222</v>
       </c>
+      <c r="G3" s="1">
+        <v>500</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>619</v>
+      </c>
       <c r="U3" s="4" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
       <c r="V3" s="4" t="s">
         <v>27</v>
@@ -2622,28 +2710,46 @@
     </row>
     <row r="4" spans="1:22" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="D4" s="4">
         <v>2023</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>621</v>
+        <v>221</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>222</v>
       </c>
+      <c r="G4" s="1">
+        <v>600</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="5" spans="1:22" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D5" s="4">
         <v>2023</v>
       </c>
@@ -2653,159 +2759,171 @@
       <c r="F5" s="1" t="s">
         <v>222</v>
       </c>
+      <c r="G5" s="1">
+        <v>700</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="6" spans="1:22" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="D6" s="4">
         <v>2023</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H6" s="1">
+        <v>1500</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="7" spans="1:22" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="D7" s="4">
         <v>2023</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H7" s="1">
+        <v>200</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>626</v>
+      </c>
     </row>
     <row r="8" spans="1:22" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="D8" s="4">
         <v>2023</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="4">
-        <v>2023</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>614</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="4">
-        <v>2023</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="4">
-        <v>2023</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="H8" s="1">
+        <v>3000</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="J8" s="1">
+        <v>4141</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L8" s="1">
+        <v>5424</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N8" s="1">
+        <v>4525</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="P8" s="1">
+        <v>2540</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R8" s="1">
+        <v>5242</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="U8" s="4" t="s">
         <v>616</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="4">
-        <v>2023</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>617</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="4">
-        <v>2023</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>618</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="4">
-        <v>2023</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>222</v>
-      </c>
+      <c r="V8" s="1" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -4477,45 +4595,50 @@
     <row r="1682" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="1683" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="G2:G1683">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>$F2 &lt;&gt; "Consumption "</formula>
+  <conditionalFormatting sqref="G3:G1683">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>$F3 &lt;&gt; "Consumption "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:I1683">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$F2 &lt;&gt; "Total Spend"</formula>
+  <conditionalFormatting sqref="H3:I1683">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$F3 &lt;&gt; "Total Spend"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:T1683">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="J3:S7 J9:S1683 J2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$E2 &lt;&gt;"Own supplier mix"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J8:S8">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$E8 &lt;&gt;"Own supplier mix"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1683" xr:uid="{4CE175D7-6AAE-4B68-88D2-189511C763EA}">
-      <formula1>"estimated, actual"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{C43CFC32-375D-4D08-A68E-496C4FF48770}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576" xr:uid="{C43CFC32-375D-4D08-A68E-496C4FF48770}">
       <formula1>"Grid average,Renewable procurement,Own supplier mix"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:T1683" xr:uid="{370297D1-A668-48D3-88C3-1E6C8442072C}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1683 K3:L1683 M2:M1683 N3:S1683" xr:uid="{370297D1-A668-48D3-88C3-1E6C8442072C}">
       <formula1>$E2 = "Own supplier mix"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{3DD7954C-A969-4DBB-9DC8-21E8D637BF3E}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F1048576" xr:uid="{3DD7954C-A969-4DBB-9DC8-21E8D637BF3E}">
       <formula1>"Consumption ,Total Spend"</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{6D0C7ABD-820C-49E0-8F25-03AECE7E379E}">
-      <formula1>$F2 = "Total Spend"</formula1>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576" xr:uid="{6D0C7ABD-820C-49E0-8F25-03AECE7E379E}">
+      <formula1>$F3 = "Total Spend"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{3A5B787E-0D19-4940-AE0C-9FAA82DB5277}">
-      <formula1>$F2 = "Consumption "</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G1048576" xr:uid="{3A5B787E-0D19-4940-AE0C-9FAA82DB5277}">
+      <formula1>$F3 = "Consumption "</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{C0C9F756-52F5-4A10-896A-34567A69185C}">
       <formula1>"Purchased Electricity"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576" xr:uid="{295C801B-53DC-4D35-B6E6-CAF9A63BD3BC}">
       <formula1>2020</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T3:T1048576" xr:uid="{6429D68C-FA31-4A7E-ADC4-A4150EA8A258}">
+      <formula1>"actual,estimated"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4530,13 +4653,13 @@
           <x14:formula1>
             <xm:f>'Conversion To Usd'!$C$2:$C$182</xm:f>
           </x14:formula1>
-          <xm:sqref>I1684:J1048576 I2:I1683</xm:sqref>
+          <xm:sqref>I3:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Country " prompt="Please select your country_x000a_" xr:uid="{AE621255-EB2D-4A5C-8372-089A2A5DD48E}">
           <x14:formula1>
             <xm:f>IEA!$A$2:$A$529</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
+          <xm:sqref>C3:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -22044,6 +22167,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="952decf2-c70e-41dd-b7af-a901e5274ebc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100316A6B2706F22F479EB96B4E836A2AA9" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb14f50e3c0e0698014ac1b2b11cfd92">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="952decf2-c70e-41dd-b7af-a901e5274ebc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e289b93c4a0db376190258ac9ef1386" ns3:_="">
     <xsd:import namespace="952decf2-c70e-41dd-b7af-a901e5274ebc"/>
@@ -22199,24 +22339,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42DCEE11-C2D1-41E8-9853-F3E1FBDDEFD7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="952decf2-c70e-41dd-b7af-a901e5274ebc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="952decf2-c70e-41dd-b7af-a901e5274ebc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAA372D8-274E-458B-B278-E3377AB6855B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F0DA129-3234-41F7-A2DE-1B7617DF62C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22232,22 +22373,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAA372D8-274E-458B-B278-E3377AB6855B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42DCEE11-C2D1-41E8-9853-F3E1FBDDEFD7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="952decf2-c70e-41dd-b7af-a901e5274ebc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>